<commit_message>
Added Screenshot function and Some Testcase.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Testdata.xlsx
+++ b/src/test/resources/data/Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Selenium-Framework\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA751B4-95E2-4278-B46C-EC9D8E5B3847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9B765F-EC76-4443-A4FD-9A250057D8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1898" yWindow="1898" windowWidth="18851" windowHeight="9766" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,6 +73,9 @@
     <t>Check-out Date</t>
   </si>
   <si>
+    <t>2023-10-15</t>
+  </si>
+  <si>
     <t>Number of Persons (Adult)</t>
   </si>
   <si>
@@ -82,10 +85,7 @@
     <t>Goa</t>
   </si>
   <si>
-    <t>2023-12-15</t>
-  </si>
-  <si>
-    <t>2024-12-20</t>
+    <t>2023-12-20</t>
   </si>
   <si>
     <t>Number of rooms</t>
@@ -525,7 +525,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -552,10 +552,10 @@
         <v>14</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>20</v>
@@ -566,10 +566,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Added allure config and some testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Testdata.xlsx
+++ b/src/test/resources/data/Testdata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Selenium-Framework\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9B765F-EC76-4443-A4FD-9A250057D8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC0A1A0-AC95-4C5B-9E95-8C2657795ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1898" yWindow="1898" windowWidth="18851" windowHeight="9766" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="759" yWindow="759" windowWidth="18851" windowHeight="9766" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
     <sheet name="Booking" sheetId="2" r:id="rId2"/>
+    <sheet name="flight" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>TestcaseName</t>
   </si>
@@ -89,6 +90,12 @@
   </si>
   <si>
     <t>Number of rooms</t>
+  </si>
+  <si>
+    <t>addDestination</t>
+  </si>
+  <si>
+    <t>nagpur</t>
   </si>
 </sst>
 </file>
@@ -524,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF660479-1369-4DCB-BBCA-38678929A24C}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -588,4 +595,56 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3891C5-D90F-4551-9EF0-AB9BB62DE5DC}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="43.85" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>